<commit_message>
Update values for future energy density of batteries
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-battery-capacity.xlsx
+++ b/premise/data/additional_inventories/lci-battery-capacity.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63122578-E956-8340-A2CA-9101DE7C0366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9DBF26-6B68-E542-88B1-5FB0F644590B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36560" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="500" windowWidth="23320" windowHeight="23000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery - NMC" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Battery - NMC'!$A$1:$H$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Battery - NMC'!$A$1:$H$170</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="92">
   <si>
     <t>Activity</t>
   </si>
@@ -88,9 +88,6 @@
     <t>kilowatt hour</t>
   </si>
   <si>
-    <t>categories</t>
-  </si>
-  <si>
     <t>database</t>
   </si>
   <si>
@@ -205,15 +202,6 @@
     <t>This dataset provides 1 kWh of battery gross capacity (NOT net), using a Li-ion LFP battery. Specific energy density in 2020: 0.14 kWh/kg cell. Battery management (BoP) mass share: 27%. Battery energy density in 2020: 0.10 kWh/kg battery. Battery mass per kWh: 9.8 kg. Lifetime: 3'000-10'000 cycles.</t>
   </si>
   <si>
-    <t>This dataset provides 1 kWh of battery gross capacity (NOT net), using a Li-ion NMC111 battery. Specific energy density in 2020: 0.197 kWh/kg cell. Battery management (BoP) mass share: 27%. Battery energy density in 2020: 0.14 kWh/kg battery. Battery mass per kWh: 6.95 kg. Lifetime: 3'000-5'000 cycles. Source for parameters: Crenna et al., 2021.</t>
-  </si>
-  <si>
-    <t>This dataset provides 1 kWh of battery gross capacity (NOT net), using a Li-ion NMC622 battery. Specific energy density in 2020: 0.200 kWh/kg cell. Battery management (BoP) mass share: 27%. Battery energy density in 2020: 0.15 kWh/kg battery. Battery mass per kWh: 6.85 kg. Lifetime: 3'000-5'000 cycles. Source for parameters: Crenna et al., 2021.</t>
-  </si>
-  <si>
-    <t>This dataset provides 1 kWh of battery gross capacity (not NET), using a Li-ion NMC811 battery. Specific energy density in 2020: 0.209 kWh/kg cell. Battery management (BoP) mass share: 29%. Battery energy density in 2020: 0.15 kWh/kg battery. Battery mass per kWh: 6.74 kg. Lifetime: 3'000-5'000 cycles. Source for parameters: Crenna et al., 2021.</t>
-  </si>
-  <si>
     <t>This dataset provides 1 kWh of battery gross capacity (NOT net), using a Li-ion NCA battery. Specific energy density in 2020: 0.224 kWh/kg cell. Battery management (BoP) mass share: 29.3%. Battery energy density in 2020: 0.159 kWh/kg battery. Battery mass per kWh: 6.74 kg. Lifetime: 3'000-5'000 cycles. Source for parameters: Crenna et al., 2021.</t>
   </si>
   <si>
@@ -272,12 +260,69 @@
   </si>
   <si>
     <t>battery capacity, Li-sulfur, Li-S</t>
+  </si>
+  <si>
+    <t>This dataset provides 1 kWh of battery gross capacity (NOT net), using a Li-ion NMC111 battery. Specific energy density in 2020: 0.197 kWh/kg cell. Battery management (BoP) mass share: 27%. Battery energy density in 2020: 0.144 kWh/kg battery. Battery mass per kWh: 6.95 kg. Lifetime: 3'000-5'000 cycles. Source for parameters: Crenna et al., 2021.</t>
+  </si>
+  <si>
+    <t>uncertainty type</t>
+  </si>
+  <si>
+    <t>loc</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>market for battery capacity, Li-ion, NMC523</t>
+  </si>
+  <si>
+    <t>battery capacity, Li-ion, NMC523</t>
+  </si>
+  <si>
+    <t>market for battery, Li-ion, NMC523</t>
+  </si>
+  <si>
+    <t>battery, Li-ion, NMC523</t>
+  </si>
+  <si>
+    <t>This dataset provides 1 kWh of battery gross capacity (NOT net), using a Li-ion NMC523 battery. Specific energy density in 2020: 0.205 kWh/kg cell. Battery management (BoP) mass share: 27%. Battery energy density in 2020: 0.150 kWh/kg battery. Battery mass per kWh: 6.95 kg. Lifetime: 3'000-5'000 cycles. Source for parameters: Xu, C., Dai, Q., Gaines, L. et al. Future material demand for automotive lithium-based batteries. Commun Mater 1, 99 (2020). https://doi.org/10.1038/s43246-020-00095-x</t>
+  </si>
+  <si>
+    <t>This dataset provides 1 kWh of battery gross capacity (NOT net), using a Li-ion NMC622 battery. Specific energy density in 2020: 0.210 kWh/kg cell. Battery management (BoP) mass share: 27%. Battery energy density in 2020: 0.15 kWh/kg battery. Battery mass per kWh: 6.85 kg. Lifetime: 3'000-5'000 cycles. Source for parameters: Crenna et al., 2021.</t>
+  </si>
+  <si>
+    <t>market for battery capacity, Li-ion, NMC955</t>
+  </si>
+  <si>
+    <t>battery capacity, Li-ion, NMC955</t>
+  </si>
+  <si>
+    <t>market for battery, Li-ion, NMC955</t>
+  </si>
+  <si>
+    <t>battery, Li-ion, NMC955</t>
+  </si>
+  <si>
+    <t>This dataset provides 1 kWh of battery gross capacity (not NET), using a Li-ion NMC955 battery. Specific energy density in 2020: 0.280 kWh/kg cell. Battery management (BoP) mass share: 29%. Battery energy density in 2030: 0.200 kWh/kg battery. Battery mass per kWh: 6.74 kg. Lifetime: 3'000-5'000 cycles. Source for parameters: Xu, C., Dai, Q., Gaines, L. et al. Future material demand for automotive lithium-based batteries. Commun Mater 1, 99 (2020). https://doi.org/10.1038/s43246-020-00095-x</t>
+  </si>
+  <si>
+    <t>This dataset provides 1 kWh of battery gross capacity (not NET), using a Li-ion NMC811 battery. Specific energy density in 2020: 0.225 kWh/kg cell. Battery management (BoP) mass share: 29%. Battery energy density in 2020: 0.16 kWh/kg battery. Battery mass per kWh: 6.74 kg. Lifetime: 3'000-5'000 cycles. Source for parameters: Crenna et al., 2021.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,7 +398,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -361,6 +406,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H144"/>
+  <dimension ref="A1:K170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F144" sqref="F144"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -655,31 +701,31 @@
     <col min="2" max="2" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -687,7 +733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -695,37 +741,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <f>1-0.27</f>
         <v>0.73</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -744,8 +791,23 @@
       <c r="F11" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="str">
         <f>B3</f>
         <v>market for battery capacity, Li-ion, LFP</v>
@@ -768,12 +830,13 @@
         <v>battery capacity, Li-ion, LFP</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>9.8000000000000007</v>
+        <v>19</v>
+      </c>
+      <c r="B13" s="7">
+        <f>1/(0.14*(1-27%))</f>
+        <v>9.7847358121330714</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -785,15 +848,31 @@
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" s="7">
+        <f>B13</f>
+        <v>9.7847358121330714</v>
+      </c>
+      <c r="I13" s="7">
+        <f>B13*0.75</f>
+        <v>7.3385518590998036</v>
+      </c>
+      <c r="J13" s="7">
+        <f>B13*1.25</f>
+        <v>12.230919765166339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14">
-        <v>-9.8000000000000007</v>
+        <v>68</v>
+      </c>
+      <c r="B14" s="7">
+        <f>-1*B13</f>
+        <v>-9.7847358121330714</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -805,26 +884,44 @@
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14" s="7">
+        <f>B14</f>
+        <v>-9.7847358121330714</v>
+      </c>
+      <c r="I14" s="7">
+        <f>B14*0.75</f>
+        <v>-7.3385518590998036</v>
+      </c>
+      <c r="J14" s="7">
+        <f>B14*1.25</f>
+        <v>-12.230919765166339</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -832,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -840,15 +937,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -856,21 +953,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B22">
         <f>1-0.27</f>
         <v>0.73</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -889,8 +986,23 @@
       <c r="F24" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="str">
         <f>B16</f>
         <v>market for battery capacity, Li-ion, NMC111</v>
@@ -913,9 +1025,9 @@
         <v>battery capacity, Li-ion, NMC111</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="3">
         <f>1/(0.197*73%)</f>
@@ -931,12 +1043,27 @@
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" s="7">
+        <f>B26</f>
+        <v>6.9536193588762956</v>
+      </c>
+      <c r="I26" s="7">
+        <f>B26*0.75</f>
+        <v>5.2152145191572217</v>
+      </c>
+      <c r="J26" s="7">
+        <f>B26*1.25</f>
+        <v>8.6920241985953695</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B27" s="3">
         <f>-1*B26</f>
@@ -952,26 +1079,44 @@
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27" s="7">
+        <f>B27</f>
+        <v>-6.9536193588762956</v>
+      </c>
+      <c r="I27" s="7">
+        <f>B27*0.75</f>
+        <v>-5.2152145191572217</v>
+      </c>
+      <c r="J27" s="7">
+        <f>B27*1.25</f>
+        <v>-8.6920241985953695</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -979,7 +1124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -987,15 +1132,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1003,21 +1148,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B35">
         <f>1-0.27</f>
         <v>0.73</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -1036,11 +1181,26 @@
       <c r="F37" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="str">
         <f>B29</f>
-        <v>market for battery capacity, Li-ion, NMC622</v>
+        <v>market for battery capacity, Li-ion, NMC523</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1057,16 +1217,16 @@
       </c>
       <c r="F38" t="str">
         <f>B33</f>
-        <v>battery capacity, Li-ion, NMC622</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>battery capacity, Li-ion, NMC523</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B39" s="3">
-        <f>1/(0.2*73%)</f>
-        <v>6.8493150684931514</v>
+        <f>1/(0.205*73%)</f>
+        <v>6.682258603407953</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -1078,16 +1238,31 @@
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+      <c r="H39" s="7">
+        <f>B39</f>
+        <v>6.682258603407953</v>
+      </c>
+      <c r="I39" s="7">
+        <f>B39*0.75</f>
+        <v>5.0116939525559649</v>
+      </c>
+      <c r="J39" s="7">
+        <f>B39*1.25</f>
+        <v>8.3528232542599419</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B40" s="3">
         <f>-1*B39</f>
-        <v>-6.8493150684931514</v>
+        <v>-6.682258603407953</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -1099,26 +1274,44 @@
         <v>14</v>
       </c>
       <c r="F40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="H40" s="7">
+        <f>B40</f>
+        <v>-6.682258603407953</v>
+      </c>
+      <c r="I40" s="7">
+        <f>B40*0.75</f>
+        <v>-5.0116939525559649</v>
+      </c>
+      <c r="J40" s="7">
+        <f>B40*1.25</f>
+        <v>-8.3528232542599419</v>
+      </c>
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1126,7 +1319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1134,37 +1327,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
       <c r="B47" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B48">
-        <f>1-0.29</f>
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <f>1-0.27</f>
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
@@ -1183,11 +1379,26 @@
       <c r="F50" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G50" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="str">
         <f>B42</f>
-        <v>market for battery capacity, Li-ion, NMC811</v>
+        <v>market for battery capacity, Li-ion, NMC622</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -1204,16 +1415,16 @@
       </c>
       <c r="F51" t="str">
         <f>B46</f>
-        <v>battery capacity, Li-ion, NMC811</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+        <v>battery capacity, Li-ion, NMC622</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>30</v>
       </c>
       <c r="B52" s="3">
-        <f>1/(0.209*71%)</f>
-        <v>6.7389985848102976</v>
+        <f>1/(0.21*73%)</f>
+        <v>6.5231572080887155</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -1225,16 +1436,31 @@
         <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52" s="7">
+        <f>B52</f>
+        <v>6.5231572080887155</v>
+      </c>
+      <c r="I52" s="7">
+        <f>B52*0.75</f>
+        <v>4.8923679060665366</v>
+      </c>
+      <c r="J52" s="7">
+        <f>B52*1.25</f>
+        <v>8.1539465101108952</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B53" s="3">
         <f>-1*B52</f>
-        <v>-6.7389985848102976</v>
+        <v>-6.5231572080887155</v>
       </c>
       <c r="C53" t="s">
         <v>7</v>
@@ -1246,26 +1472,44 @@
         <v>14</v>
       </c>
       <c r="F53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53" s="7">
+        <f>B53</f>
+        <v>-6.5231572080887155</v>
+      </c>
+      <c r="I53" s="7">
+        <f>B53*0.75</f>
+        <v>-4.8923679060665366</v>
+      </c>
+      <c r="J53" s="7">
+        <f>B53*1.25</f>
+        <v>-8.1539465101108952</v>
+      </c>
+      <c r="K53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -1273,7 +1517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -1281,37 +1525,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B61">
-        <f>1-0.293</f>
-        <v>0.70700000000000007</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <f>1-0.29</f>
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
@@ -1330,11 +1575,26 @@
       <c r="F63" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G63" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="str">
         <f>B55</f>
-        <v>market for battery capacity, Li-ion, NCA</v>
+        <v>market for battery capacity, Li-ion, NMC811</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1351,16 +1611,16 @@
       </c>
       <c r="F64" t="str">
         <f>B59</f>
-        <v>battery capacity, Li-ion, NCA</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+        <v>battery capacity, Li-ion, NMC811</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B65" s="3">
-        <f>1/(0.224*70.7%)</f>
-        <v>6.3144069508991709</v>
+        <f>1/(0.225*71%)</f>
+        <v>6.2597809076682314</v>
       </c>
       <c r="C65" t="s">
         <v>7</v>
@@ -1372,16 +1632,31 @@
         <v>14</v>
       </c>
       <c r="F65" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="G65">
+        <v>5</v>
+      </c>
+      <c r="H65" s="7">
+        <f>B65</f>
+        <v>6.2597809076682314</v>
+      </c>
+      <c r="I65" s="7">
+        <f>B65*0.75</f>
+        <v>4.694835680751174</v>
+      </c>
+      <c r="J65" s="7">
+        <f>B65*1.25</f>
+        <v>7.8247261345852888</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B66" s="3">
         <f>-1*B65</f>
-        <v>-6.3144069508991709</v>
+        <v>-6.2597809076682314</v>
       </c>
       <c r="C66" t="s">
         <v>7</v>
@@ -1393,26 +1668,44 @@
         <v>14</v>
       </c>
       <c r="F66" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G66">
+        <v>5</v>
+      </c>
+      <c r="H66" s="7">
+        <f>B66</f>
+        <v>-6.2597809076682314</v>
+      </c>
+      <c r="I66" s="7">
+        <f>B66*0.75</f>
+        <v>-4.694835680751174</v>
+      </c>
+      <c r="J66" s="7">
+        <f>B66*1.25</f>
+        <v>-7.8247261345852888</v>
+      </c>
+      <c r="K66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -1420,7 +1713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -1428,37 +1721,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>6</v>
       </c>
       <c r="B73" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B74">
-        <f>1-0.36</f>
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <f>1-0.29</f>
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>10</v>
       </c>
@@ -1477,11 +1771,26 @@
       <c r="F76" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="str">
+      <c r="G76" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="str">
         <f>B68</f>
-        <v>market for battery capacity, Li-ion, LTO</v>
+        <v>market for battery capacity, Li-ion, NMC955</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -1498,16 +1807,16 @@
       </c>
       <c r="F77" t="str">
         <f>B72</f>
-        <v>battery capacity, Li-ion, LTO</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+        <v>battery capacity, Li-ion, NMC955</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="B78" s="3">
-        <f>1/(0.085*64%)</f>
-        <v>18.382352941176471</v>
+        <f>1/(0.28*71%)</f>
+        <v>5.0301810865191143</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
@@ -1519,16 +1828,31 @@
         <v>14</v>
       </c>
       <c r="F78" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="G78">
+        <v>5</v>
+      </c>
+      <c r="H78" s="7">
+        <f>B78</f>
+        <v>5.0301810865191143</v>
+      </c>
+      <c r="I78" s="7">
+        <f>B78*0.75</f>
+        <v>3.7726358148893357</v>
+      </c>
+      <c r="J78" s="7">
+        <f>B78*1.25</f>
+        <v>6.2877263581488929</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B79" s="3">
         <f>-1*B78</f>
-        <v>-18.382352941176471</v>
+        <v>-5.0301810865191143</v>
       </c>
       <c r="C79" t="s">
         <v>7</v>
@@ -1540,26 +1864,44 @@
         <v>14</v>
       </c>
       <c r="F79" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G79">
+        <v>5</v>
+      </c>
+      <c r="H79" s="7">
+        <f>B79</f>
+        <v>-5.0301810865191143</v>
+      </c>
+      <c r="I79" s="7">
+        <f>B79*0.75</f>
+        <v>-3.7726358148893357</v>
+      </c>
+      <c r="J79" s="7">
+        <f>B79*1.25</f>
+        <v>-6.2877263581488929</v>
+      </c>
+      <c r="K79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>2</v>
       </c>
@@ -1567,7 +1909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -1575,37 +1917,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>6</v>
       </c>
       <c r="B86" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B87">
-        <f>1-0.13</f>
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <f>1-0.293</f>
+        <v>0.70700000000000007</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>10</v>
       </c>
@@ -1624,11 +1967,26 @@
       <c r="F89" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="6" t="str">
+      <c r="G89" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="str">
         <f>B81</f>
-        <v>market for battery capacity, Li-ion, LiMn2O4</v>
+        <v>market for battery capacity, Li-ion, NCA</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -1645,16 +2003,16 @@
       </c>
       <c r="F90" t="str">
         <f>B85</f>
-        <v>battery capacity, Li-ion, LiMn2O4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+        <v>battery capacity, Li-ion, NCA</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B91" s="3">
-        <f>1/(32/280)</f>
-        <v>8.75</v>
+        <f>1/(0.224*70.7%)</f>
+        <v>6.3144069508991709</v>
       </c>
       <c r="C91" t="s">
         <v>7</v>
@@ -1666,16 +2024,31 @@
         <v>14</v>
       </c>
       <c r="F91" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="G91">
+        <v>5</v>
+      </c>
+      <c r="H91" s="7">
+        <f>B91</f>
+        <v>6.3144069508991709</v>
+      </c>
+      <c r="I91" s="7">
+        <f>B91*0.75</f>
+        <v>4.7358052131743786</v>
+      </c>
+      <c r="J91" s="7">
+        <f>B91*1.25</f>
+        <v>7.8930086886239632</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B92" s="3">
         <f>-1*B91</f>
-        <v>-8.75</v>
+        <v>-6.3144069508991709</v>
       </c>
       <c r="C92" t="s">
         <v>7</v>
@@ -1687,26 +2060,44 @@
         <v>14</v>
       </c>
       <c r="F92" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G92">
+        <v>5</v>
+      </c>
+      <c r="H92" s="7">
+        <f>B92</f>
+        <v>-6.3144069508991709</v>
+      </c>
+      <c r="I92" s="7">
+        <f>B92*0.75</f>
+        <v>-4.7358052131743786</v>
+      </c>
+      <c r="J92" s="7">
+        <f>B92*1.25</f>
+        <v>-7.8930086886239632</v>
+      </c>
+      <c r="K92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>1</v>
       </c>
       <c r="B95" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -1714,7 +2105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>4</v>
       </c>
@@ -1722,15 +2113,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="E98" s="3"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -1738,21 +2130,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B100">
-        <f>1-0.25</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <f>1-0.36</f>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>10</v>
       </c>
@@ -1771,11 +2163,26 @@
       <c r="F102" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A103" s="4" t="str">
+      <c r="G102" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="6" t="str">
         <f>B94</f>
-        <v>market for battery capacity, Li-sulfur, Li-S</v>
+        <v>market for battery capacity, Li-ion, LTO</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -1792,16 +2199,16 @@
       </c>
       <c r="F103" t="str">
         <f>B98</f>
-        <v>battery capacity, Li-sulfur, Li-S</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+        <v>battery capacity, Li-ion, LTO</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B104" s="3">
-        <f>1/(0.15*75%)</f>
-        <v>8.8888888888888893</v>
+        <f>1/(0.085*64%)</f>
+        <v>18.382352941176471</v>
       </c>
       <c r="C104" t="s">
         <v>7</v>
@@ -1813,16 +2220,31 @@
         <v>14</v>
       </c>
       <c r="F104" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="G104">
+        <v>5</v>
+      </c>
+      <c r="H104" s="7">
+        <f>B104</f>
+        <v>18.382352941176471</v>
+      </c>
+      <c r="I104" s="7">
+        <f>B104*0.75</f>
+        <v>13.786764705882353</v>
+      </c>
+      <c r="J104" s="7">
+        <f>B104*1.25</f>
+        <v>22.977941176470587</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B105" s="3">
         <f>-1*B104</f>
-        <v>-8.8888888888888893</v>
+        <v>-18.382352941176471</v>
       </c>
       <c r="C105" t="s">
         <v>7</v>
@@ -1834,26 +2256,44 @@
         <v>14</v>
       </c>
       <c r="F105" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G105">
+        <v>5</v>
+      </c>
+      <c r="H105" s="7">
+        <f>B105</f>
+        <v>-18.382352941176471</v>
+      </c>
+      <c r="I105" s="7">
+        <f>B105*0.75</f>
+        <v>-13.786764705882353</v>
+      </c>
+      <c r="J105" s="7">
+        <f>B105*1.25</f>
+        <v>-22.977941176470587</v>
+      </c>
+      <c r="K105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>1</v>
       </c>
       <c r="B108" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>2</v>
       </c>
@@ -1861,7 +2301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>4</v>
       </c>
@@ -1869,37 +2309,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>5</v>
       </c>
       <c r="B111" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>6</v>
       </c>
       <c r="B112" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E112" s="3"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B113">
-        <f>1-0.45</f>
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <f>1-0.13</f>
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>10</v>
       </c>
@@ -1918,11 +2359,26 @@
       <c r="F115" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="str">
+      <c r="G115" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="6" t="str">
         <f>B107</f>
-        <v>market for battery capacity, Li-ion, Li-O2</v>
+        <v>market for battery capacity, Li-ion, LiMn2O4</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -1939,16 +2395,16 @@
       </c>
       <c r="F116" t="str">
         <f>B111</f>
-        <v>battery capacity, Li-ion, Li-O2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+        <v>battery capacity, Li-ion, LiMn2O4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B117" s="3">
-        <f>1/0.198</f>
-        <v>5.0505050505050502</v>
+        <f>1/(32/280)</f>
+        <v>8.75</v>
       </c>
       <c r="C117" t="s">
         <v>7</v>
@@ -1960,16 +2416,31 @@
         <v>14</v>
       </c>
       <c r="F117" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="G117">
+        <v>5</v>
+      </c>
+      <c r="H117" s="7">
+        <f>B117</f>
+        <v>8.75</v>
+      </c>
+      <c r="I117" s="7">
+        <f>B117*0.75</f>
+        <v>6.5625</v>
+      </c>
+      <c r="J117" s="7">
+        <f>B117*1.25</f>
+        <v>10.9375</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B118" s="3">
         <f>-1*B117</f>
-        <v>-5.0505050505050502</v>
+        <v>-8.75</v>
       </c>
       <c r="C118" t="s">
         <v>7</v>
@@ -1981,26 +2452,44 @@
         <v>14</v>
       </c>
       <c r="F118" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G118">
+        <v>5</v>
+      </c>
+      <c r="H118" s="7">
+        <f>B118</f>
+        <v>-8.75</v>
+      </c>
+      <c r="I118" s="7">
+        <f>B118*0.75</f>
+        <v>-6.5625</v>
+      </c>
+      <c r="J118" s="7">
+        <f>B118*1.25</f>
+        <v>-10.9375</v>
+      </c>
+      <c r="K118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>1</v>
       </c>
       <c r="B121" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>2</v>
       </c>
@@ -2008,7 +2497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>4</v>
       </c>
@@ -2016,37 +2505,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>5</v>
       </c>
       <c r="B124" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>6</v>
       </c>
       <c r="B125" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D125" s="3"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B126">
         <f>1-0.25</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>10</v>
       </c>
@@ -2065,11 +2555,26 @@
       <c r="F128" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="G128" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="str">
         <f>B120</f>
-        <v>market for battery capacity, Sodium-ion, SiB</v>
+        <v>market for battery capacity, Li-sulfur, Li-S</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2086,211 +2591,677 @@
       </c>
       <c r="F129" t="str">
         <f>B124</f>
+        <v>battery capacity, Li-sulfur, Li-S</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>41</v>
+      </c>
+      <c r="B130" s="3">
+        <f>1/(0.15*75%)</f>
+        <v>8.8888888888888893</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130" t="s">
+        <v>3</v>
+      </c>
+      <c r="E130" t="s">
+        <v>14</v>
+      </c>
+      <c r="F130" t="s">
+        <v>42</v>
+      </c>
+      <c r="G130">
+        <v>5</v>
+      </c>
+      <c r="H130" s="7">
+        <f>B130</f>
+        <v>8.8888888888888893</v>
+      </c>
+      <c r="I130" s="7">
+        <f>B130*0.75</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="J130" s="7">
+        <f>B130*1.25</f>
+        <v>11.111111111111111</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>68</v>
+      </c>
+      <c r="B131" s="3">
+        <f>-1*B130</f>
+        <v>-8.8888888888888893</v>
+      </c>
+      <c r="C131" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" t="s">
+        <v>3</v>
+      </c>
+      <c r="E131" t="s">
+        <v>14</v>
+      </c>
+      <c r="F131" t="s">
+        <v>69</v>
+      </c>
+      <c r="G131">
+        <v>5</v>
+      </c>
+      <c r="H131" s="7">
+        <f>B131</f>
+        <v>-8.8888888888888893</v>
+      </c>
+      <c r="I131" s="7">
+        <f>B131*0.75</f>
+        <v>-6.666666666666667</v>
+      </c>
+      <c r="J131" s="7">
+        <f>B131*1.25</f>
+        <v>-11.111111111111111</v>
+      </c>
+      <c r="K131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A133" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>1</v>
+      </c>
+      <c r="B134" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B135" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>4</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>5</v>
+      </c>
+      <c r="B137" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>6</v>
+      </c>
+      <c r="B138" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>60</v>
+      </c>
+      <c r="B139">
+        <f>1-0.45</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J141" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A142" s="4" t="str">
+        <f>B133</f>
+        <v>market for battery capacity, Li-ion, Li-O2</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142" t="str">
+        <f>B138</f>
+        <v>kilowatt hour</v>
+      </c>
+      <c r="D142" t="s">
+        <v>3</v>
+      </c>
+      <c r="E142" t="s">
+        <v>13</v>
+      </c>
+      <c r="F142" t="str">
+        <f>B137</f>
+        <v>battery capacity, Li-ion, Li-O2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>45</v>
+      </c>
+      <c r="B143" s="3">
+        <f>1/0.198</f>
+        <v>5.0505050505050502</v>
+      </c>
+      <c r="C143" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" t="s">
+        <v>3</v>
+      </c>
+      <c r="E143" t="s">
+        <v>14</v>
+      </c>
+      <c r="F143" t="s">
+        <v>46</v>
+      </c>
+      <c r="G143">
+        <v>5</v>
+      </c>
+      <c r="H143" s="7">
+        <f>B143</f>
+        <v>5.0505050505050502</v>
+      </c>
+      <c r="I143" s="7">
+        <f>B143*0.75</f>
+        <v>3.7878787878787876</v>
+      </c>
+      <c r="J143" s="7">
+        <f>B143*1.25</f>
+        <v>6.3131313131313131</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>68</v>
+      </c>
+      <c r="B144" s="3">
+        <f>-1*B143</f>
+        <v>-5.0505050505050502</v>
+      </c>
+      <c r="C144" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144" t="s">
+        <v>3</v>
+      </c>
+      <c r="E144" t="s">
+        <v>14</v>
+      </c>
+      <c r="F144" t="s">
+        <v>69</v>
+      </c>
+      <c r="G144">
+        <v>5</v>
+      </c>
+      <c r="H144" s="7">
+        <f>B144</f>
+        <v>-5.0505050505050502</v>
+      </c>
+      <c r="I144" s="7">
+        <f>B144*0.75</f>
+        <v>-3.7878787878787876</v>
+      </c>
+      <c r="J144" s="7">
+        <f>B144*1.25</f>
+        <v>-6.3131313131313131</v>
+      </c>
+      <c r="K144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>1</v>
+      </c>
+      <c r="B147" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>2</v>
+      </c>
+      <c r="B148" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>4</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>5</v>
+      </c>
+      <c r="B150" t="s">
+        <v>50</v>
+      </c>
+      <c r="E150" s="3"/>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>6</v>
+      </c>
+      <c r="B151" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>60</v>
+      </c>
+      <c r="B152">
+        <f>1-0.25</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I154" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J154" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K154" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A155" s="4" t="str">
+        <f>B146</f>
+        <v>market for battery capacity, Sodium-ion, SiB</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155" t="str">
+        <f>B151</f>
+        <v>kilowatt hour</v>
+      </c>
+      <c r="D155" t="s">
+        <v>3</v>
+      </c>
+      <c r="E155" t="s">
+        <v>13</v>
+      </c>
+      <c r="F155" t="str">
+        <f>B150</f>
         <v>battery capacity, Sodium-ion, SiB</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>49</v>
-      </c>
-      <c r="B130" s="3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>48</v>
+      </c>
+      <c r="B156" s="3">
         <f>1/(0.157*75%)</f>
         <v>8.4925690021231421</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C156" t="s">
         <v>7</v>
       </c>
-      <c r="D130" t="s">
-        <v>3</v>
-      </c>
-      <c r="E130" t="s">
+      <c r="D156" t="s">
+        <v>3</v>
+      </c>
+      <c r="E156" t="s">
         <v>14</v>
       </c>
-      <c r="F130" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>72</v>
-      </c>
-      <c r="B131" s="3">
-        <f>-1*B130</f>
+      <c r="F156" t="s">
+        <v>49</v>
+      </c>
+      <c r="G156">
+        <v>5</v>
+      </c>
+      <c r="H156" s="7">
+        <f>B156</f>
+        <v>8.4925690021231421</v>
+      </c>
+      <c r="I156" s="7">
+        <f>B156*0.75</f>
+        <v>6.369426751592357</v>
+      </c>
+      <c r="J156" s="7">
+        <f>B156*1.25</f>
+        <v>10.615711252653927</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>68</v>
+      </c>
+      <c r="B157" s="3">
+        <f>-1*B156</f>
         <v>-8.4925690021231421</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C157" t="s">
         <v>7</v>
       </c>
-      <c r="D131" t="s">
-        <v>3</v>
-      </c>
-      <c r="E131" t="s">
+      <c r="D157" t="s">
+        <v>3</v>
+      </c>
+      <c r="E157" t="s">
         <v>14</v>
       </c>
-      <c r="F131" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A133" s="2" t="s">
+      <c r="F157" t="s">
+        <v>69</v>
+      </c>
+      <c r="G157">
+        <v>5</v>
+      </c>
+      <c r="H157" s="7">
+        <f>B157</f>
+        <v>-8.4925690021231421</v>
+      </c>
+      <c r="I157" s="7">
+        <f>B157*0.75</f>
+        <v>-6.369426751592357</v>
+      </c>
+      <c r="J157" s="7">
+        <f>B157*1.25</f>
+        <v>-10.615711252653927</v>
+      </c>
+      <c r="K157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>1</v>
-      </c>
-      <c r="B134" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="B159" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>1</v>
+      </c>
+      <c r="B160" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>2</v>
       </c>
-      <c r="B135" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+      <c r="B161" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>4</v>
       </c>
-      <c r="B136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>5</v>
-      </c>
-      <c r="B137" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>5</v>
+      </c>
+      <c r="B163" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
         <v>6</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B164" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>8</v>
       </c>
-      <c r="B139" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
+      <c r="B165" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B140" s="1"/>
-      <c r="C140" s="1"/>
-      <c r="D140" s="1"/>
-      <c r="E140" s="1"/>
-      <c r="F140" s="1"/>
-      <c r="G140" s="1"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="1"/>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B167" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C167" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E141" s="1" t="s">
+      <c r="D167" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F141" s="1" t="s">
+      <c r="E167" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G141" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H141" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A142" s="5" t="str">
-        <f>B133</f>
+      <c r="F167" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I167" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J167" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K167" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A168" s="5" t="str">
+        <f>B159</f>
         <v>market for battery capacity, Sodium-Nickel-Chloride, Na-NiCl</v>
       </c>
-      <c r="B142">
-        <v>1</v>
-      </c>
-      <c r="C142" t="s">
+      <c r="B168">
+        <v>1</v>
+      </c>
+      <c r="C168" t="s">
         <v>15</v>
       </c>
-      <c r="E142" t="str">
-        <f>B135</f>
+      <c r="D168" t="str">
+        <f>B161</f>
         <v>GLO</v>
       </c>
-      <c r="F142" t="s">
+      <c r="E168" t="s">
         <v>13</v>
       </c>
-      <c r="G142" t="str">
-        <f>B137</f>
+      <c r="F168" t="str">
+        <f>B163</f>
         <v>battery capacity, Na-NiCl</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>52</v>
-      </c>
-      <c r="B143" s="3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>51</v>
+      </c>
+      <c r="B169" s="3">
         <f>1/0.116</f>
         <v>8.6206896551724128</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C169" t="s">
         <v>7</v>
       </c>
-      <c r="E143" t="s">
-        <v>3</v>
-      </c>
-      <c r="F143" t="s">
+      <c r="D169" t="s">
+        <v>3</v>
+      </c>
+      <c r="E169" t="s">
         <v>14</v>
       </c>
-      <c r="G143" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>72</v>
-      </c>
-      <c r="B144" s="3">
-        <f>-1*B143</f>
+      <c r="F169" t="s">
+        <v>52</v>
+      </c>
+      <c r="G169">
+        <v>5</v>
+      </c>
+      <c r="H169" s="7">
+        <f>B169</f>
+        <v>8.6206896551724128</v>
+      </c>
+      <c r="I169" s="7">
+        <f>B169*0.75</f>
+        <v>6.4655172413793096</v>
+      </c>
+      <c r="J169" s="7">
+        <f>B169*1.25</f>
+        <v>10.775862068965516</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>68</v>
+      </c>
+      <c r="B170" s="3">
+        <f>-1*B169</f>
         <v>-8.6206896551724128</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C170" t="s">
         <v>7</v>
       </c>
-      <c r="E144" t="s">
-        <v>3</v>
-      </c>
-      <c r="F144" t="s">
+      <c r="D170" t="s">
+        <v>3</v>
+      </c>
+      <c r="E170" t="s">
         <v>14</v>
       </c>
-      <c r="G144" t="s">
-        <v>73</v>
+      <c r="F170" t="s">
+        <v>69</v>
+      </c>
+      <c r="G170">
+        <v>5</v>
+      </c>
+      <c r="H170" s="7">
+        <f>B170</f>
+        <v>-8.6206896551724128</v>
+      </c>
+      <c r="I170" s="7">
+        <f>B170*0.75</f>
+        <v>-6.4655172413793096</v>
+      </c>
+      <c r="J170" s="7">
+        <f>B170*1.25</f>
+        <v>-10.775862068965516</v>
+      </c>
+      <c r="K170" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H144" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H170" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjust truck battery size
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-battery-capacity.xlsx
+++ b/premise/data/additional_inventories/lci-battery-capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4290815-5539-434A-B68F-C88551189D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929081F9-5788-7C44-B5A7-717DC169D6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1040" windowWidth="25600" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery - NMC" sheetId="1" r:id="rId1"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N266"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="J157" sqref="J157"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="A248" sqref="A248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3491,7 +3491,7 @@
         <v>16</v>
       </c>
       <c r="B182">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C182" t="s">
         <v>15</v>
@@ -3531,7 +3531,7 @@
         <v>62</v>
       </c>
       <c r="B184">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C184" t="s">
         <v>15</v>
@@ -3551,7 +3551,7 @@
         <v>22</v>
       </c>
       <c r="B185">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C185" t="s">
         <v>15</v>
@@ -3571,7 +3571,7 @@
         <v>23</v>
       </c>
       <c r="B186">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C186" t="s">
         <v>15</v>
@@ -3611,7 +3611,7 @@
         <v>27</v>
       </c>
       <c r="B188">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="C188" t="s">
         <v>15</v>
@@ -3869,7 +3869,7 @@
         <v>16</v>
       </c>
       <c r="B206">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C206" t="s">
         <v>15</v>
@@ -3909,7 +3909,7 @@
         <v>62</v>
       </c>
       <c r="B208">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C208" t="s">
         <v>15</v>
@@ -3929,7 +3929,7 @@
         <v>22</v>
       </c>
       <c r="B209">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C209" t="s">
         <v>15</v>
@@ -3949,7 +3949,7 @@
         <v>23</v>
       </c>
       <c r="B210">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C210" t="s">
         <v>15</v>
@@ -3989,7 +3989,7 @@
         <v>27</v>
       </c>
       <c r="B212">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="C212" t="s">
         <v>15</v>
@@ -4247,7 +4247,7 @@
         <v>16</v>
       </c>
       <c r="B230">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C230" t="s">
         <v>15</v>
@@ -4287,7 +4287,7 @@
         <v>62</v>
       </c>
       <c r="B232">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C232" t="s">
         <v>15</v>
@@ -4307,7 +4307,7 @@
         <v>22</v>
       </c>
       <c r="B233">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C233" t="s">
         <v>15</v>
@@ -4327,7 +4327,7 @@
         <v>23</v>
       </c>
       <c r="B234">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C234" t="s">
         <v>15</v>
@@ -4367,7 +4367,7 @@
         <v>27</v>
       </c>
       <c r="B236">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="C236" t="s">
         <v>15</v>
@@ -4625,7 +4625,7 @@
         <v>16</v>
       </c>
       <c r="B254">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C254" t="s">
         <v>15</v>
@@ -4665,7 +4665,7 @@
         <v>62</v>
       </c>
       <c r="B256">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C256" t="s">
         <v>15</v>
@@ -4685,7 +4685,7 @@
         <v>22</v>
       </c>
       <c r="B257">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C257" t="s">
         <v>15</v>
@@ -4705,7 +4705,7 @@
         <v>23</v>
       </c>
       <c r="B258">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C258" t="s">
         <v>15</v>
@@ -4745,7 +4745,7 @@
         <v>27</v>
       </c>
       <c r="B260">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="C260" t="s">
         <v>15</v>
@@ -4891,8 +4891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E327F433-64CA-4C75-A0BC-FFEEC2922B0D}">
   <dimension ref="A1:N203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="J120" sqref="J120"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7038,7 +7038,7 @@
         <v>83</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C145" t="s">
         <v>15</v>
@@ -7058,7 +7058,7 @@
         <v>84</v>
       </c>
       <c r="B146">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="C146" t="s">
         <v>15</v>
@@ -7098,7 +7098,7 @@
         <v>86</v>
       </c>
       <c r="B148">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="C148" t="s">
         <v>15</v>
@@ -7118,7 +7118,7 @@
         <v>87</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="C149" t="s">
         <v>15</v>
@@ -7178,7 +7178,7 @@
         <v>106</v>
       </c>
       <c r="B152">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C152" t="s">
         <v>15</v>
@@ -7198,7 +7198,7 @@
         <v>94</v>
       </c>
       <c r="B153" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C153" t="s">
         <v>15</v>
@@ -7223,7 +7223,7 @@
         <v>100</v>
       </c>
       <c r="B154">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C154" t="s">
         <v>15</v>
@@ -7362,7 +7362,7 @@
         <v>83</v>
       </c>
       <c r="B166">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C166" t="s">
         <v>15</v>
@@ -7382,7 +7382,7 @@
         <v>84</v>
       </c>
       <c r="B167">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="C167" t="s">
         <v>15</v>
@@ -7422,7 +7422,7 @@
         <v>86</v>
       </c>
       <c r="B169">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="C169" t="s">
         <v>15</v>
@@ -7442,7 +7442,7 @@
         <v>87</v>
       </c>
       <c r="B170">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="C170" t="s">
         <v>15</v>
@@ -7502,7 +7502,7 @@
         <v>106</v>
       </c>
       <c r="B173">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C173" t="s">
         <v>15</v>
@@ -7522,7 +7522,7 @@
         <v>94</v>
       </c>
       <c r="B174" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C174" t="s">
         <v>15</v>
@@ -7544,7 +7544,7 @@
         <v>100</v>
       </c>
       <c r="B175">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C175" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Fix linking issues with ei37
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-battery-capacity.xlsx
+++ b/premise/data/additional_inventories/lci-battery-capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929081F9-5788-7C44-B5A7-717DC169D6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4290815-5539-434A-B68F-C88551189D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1040" windowWidth="25600" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery - NMC" sheetId="1" r:id="rId1"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="A248" sqref="A248"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="J157" sqref="J157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3491,7 +3491,7 @@
         <v>16</v>
       </c>
       <c r="B182">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="C182" t="s">
         <v>15</v>
@@ -3531,7 +3531,7 @@
         <v>62</v>
       </c>
       <c r="B184">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C184" t="s">
         <v>15</v>
@@ -3551,7 +3551,7 @@
         <v>22</v>
       </c>
       <c r="B185">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C185" t="s">
         <v>15</v>
@@ -3571,7 +3571,7 @@
         <v>23</v>
       </c>
       <c r="B186">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C186" t="s">
         <v>15</v>
@@ -3611,7 +3611,7 @@
         <v>27</v>
       </c>
       <c r="B188">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="C188" t="s">
         <v>15</v>
@@ -3869,7 +3869,7 @@
         <v>16</v>
       </c>
       <c r="B206">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="C206" t="s">
         <v>15</v>
@@ -3909,7 +3909,7 @@
         <v>62</v>
       </c>
       <c r="B208">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C208" t="s">
         <v>15</v>
@@ -3929,7 +3929,7 @@
         <v>22</v>
       </c>
       <c r="B209">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C209" t="s">
         <v>15</v>
@@ -3949,7 +3949,7 @@
         <v>23</v>
       </c>
       <c r="B210">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C210" t="s">
         <v>15</v>
@@ -3989,7 +3989,7 @@
         <v>27</v>
       </c>
       <c r="B212">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="C212" t="s">
         <v>15</v>
@@ -4247,7 +4247,7 @@
         <v>16</v>
       </c>
       <c r="B230">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="C230" t="s">
         <v>15</v>
@@ -4287,7 +4287,7 @@
         <v>62</v>
       </c>
       <c r="B232">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C232" t="s">
         <v>15</v>
@@ -4307,7 +4307,7 @@
         <v>22</v>
       </c>
       <c r="B233">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C233" t="s">
         <v>15</v>
@@ -4327,7 +4327,7 @@
         <v>23</v>
       </c>
       <c r="B234">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C234" t="s">
         <v>15</v>
@@ -4367,7 +4367,7 @@
         <v>27</v>
       </c>
       <c r="B236">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="C236" t="s">
         <v>15</v>
@@ -4625,7 +4625,7 @@
         <v>16</v>
       </c>
       <c r="B254">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="C254" t="s">
         <v>15</v>
@@ -4665,7 +4665,7 @@
         <v>62</v>
       </c>
       <c r="B256">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C256" t="s">
         <v>15</v>
@@ -4685,7 +4685,7 @@
         <v>22</v>
       </c>
       <c r="B257">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C257" t="s">
         <v>15</v>
@@ -4705,7 +4705,7 @@
         <v>23</v>
       </c>
       <c r="B258">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="C258" t="s">
         <v>15</v>
@@ -4745,7 +4745,7 @@
         <v>27</v>
       </c>
       <c r="B260">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="C260" t="s">
         <v>15</v>
@@ -4891,8 +4891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E327F433-64CA-4C75-A0BC-FFEEC2922B0D}">
   <dimension ref="A1:N203"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="J120" sqref="J120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7038,7 +7038,7 @@
         <v>83</v>
       </c>
       <c r="B145">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C145" t="s">
         <v>15</v>
@@ -7058,7 +7058,7 @@
         <v>84</v>
       </c>
       <c r="B146">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="C146" t="s">
         <v>15</v>
@@ -7098,7 +7098,7 @@
         <v>86</v>
       </c>
       <c r="B148">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="C148" t="s">
         <v>15</v>
@@ -7118,7 +7118,7 @@
         <v>87</v>
       </c>
       <c r="B149">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="C149" t="s">
         <v>15</v>
@@ -7178,7 +7178,7 @@
         <v>106</v>
       </c>
       <c r="B152">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C152" t="s">
         <v>15</v>
@@ -7198,7 +7198,7 @@
         <v>94</v>
       </c>
       <c r="B153" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C153" t="s">
         <v>15</v>
@@ -7223,7 +7223,7 @@
         <v>100</v>
       </c>
       <c r="B154">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C154" t="s">
         <v>15</v>
@@ -7362,7 +7362,7 @@
         <v>83</v>
       </c>
       <c r="B166">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C166" t="s">
         <v>15</v>
@@ -7382,7 +7382,7 @@
         <v>84</v>
       </c>
       <c r="B167">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="C167" t="s">
         <v>15</v>
@@ -7422,7 +7422,7 @@
         <v>86</v>
       </c>
       <c r="B169">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="C169" t="s">
         <v>15</v>
@@ -7442,7 +7442,7 @@
         <v>87</v>
       </c>
       <c r="B170">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="C170" t="s">
         <v>15</v>
@@ -7502,7 +7502,7 @@
         <v>106</v>
       </c>
       <c r="B173">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C173" t="s">
         <v>15</v>
@@ -7522,7 +7522,7 @@
         <v>94</v>
       </c>
       <c r="B174" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C174" t="s">
         <v>15</v>
@@ -7544,7 +7544,7 @@
         <v>100</v>
       </c>
       <c r="B175">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C175" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Add electricity input to "electricity supply, from stationary battery (CONT scenario)"
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-battery-capacity.xlsx
+++ b/premise/data/additional_inventories/lci-battery-capacity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDE3F92-10D4-6F4D-8BAF-167EB7E4E18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F695C9D6-308E-D943-95CD-FA6782439EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37440" yWindow="400" windowWidth="25600" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="116">
   <si>
     <t>Activity</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>market for battery capacity, Li-ion, NMC532, stationary</t>
+  </si>
+  <si>
+    <t>Loss</t>
   </si>
 </sst>
 </file>
@@ -4892,8 +4895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E327F433-64CA-4C75-A0BC-FFEEC2922B0D}">
   <dimension ref="A1:N203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H190" sqref="H190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7670,7 +7673,9 @@
       <c r="J185" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K185" s="1"/>
+      <c r="K185" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" t="str">
@@ -7768,19 +7773,32 @@
       <c r="J188">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A189" s="1"/>
-      <c r="B189" s="1"/>
-      <c r="C189" s="1"/>
-      <c r="D189" s="1"/>
-      <c r="E189" s="1"/>
-      <c r="F189" s="1"/>
-      <c r="G189" s="1"/>
-      <c r="H189" s="1"/>
-      <c r="I189" s="1"/>
-      <c r="J189" s="1"/>
-      <c r="K189" s="1"/>
+      <c r="K188" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A189" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
+      <c r="C189" t="s">
+        <v>15</v>
+      </c>
+      <c r="D189" t="s">
+        <v>3</v>
+      </c>
+      <c r="E189" t="s">
+        <v>14</v>
+      </c>
+      <c r="F189" t="s">
+        <v>104</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G190" s="1"/>

</xml_diff>